<commit_message>
Weight & CG Estimation Code
Coding part is finished, actual design parameter is acquired
</commit_message>
<xml_diff>
--- a/conceptual design review/sections/VIII - weight and balance/B_Required_Data.xlsx
+++ b/conceptual design review/sections/VIII - weight and balance/B_Required_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/hl3422_ic_ac_uk/Documents/Year 3/Aerospace Vehicle Design/G - GitHub/AVD/conceptual design review/sections/VIII - weight and balance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2116" documentId="11_AD4DA82427541F7ACA7EB805C8CF33D06AE8DE11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6267468D-7593-4C30-8390-400EB07F9EB2}"/>
+  <xr:revisionPtr revIDLastSave="2117" documentId="11_AD4DA82427541F7ACA7EB805C8CF33D06AE8DE11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{639C2920-CFD0-4AD8-A24E-6FB338779DDE}"/>
   <bookViews>
     <workbookView xWindow="21840" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="442">
   <si>
     <t>Parameter</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2010,6 +2010,10 @@
   </si>
   <si>
     <t>63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2247,6 +2251,30 @@
     <xf numFmtId="176" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2254,18 +2282,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2274,52 +2305,25 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2619,32 +2623,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="40" t="s">
         <v>200</v>
       </c>
     </row>
@@ -2661,22 +2665,22 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
@@ -2799,17 +2803,17 @@
       <c r="G10" s="36"/>
     </row>
     <row r="11" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -3005,7 +3009,7 @@
       <c r="E20" s="13">
         <v>0.13</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="22">
         <v>0.16</v>
       </c>
       <c r="G20" s="13">
@@ -3099,17 +3103,17 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="23" t="s">
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -3280,17 +3284,17 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="23" t="s">
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
@@ -3419,17 +3423,17 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="23" t="s">
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
     </row>
     <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
@@ -3537,17 +3541,17 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="22" t="s">
+      <c r="A47" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="23" t="s">
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
     </row>
     <row r="48" spans="1:7" ht="36" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
@@ -3700,17 +3704,17 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="22" t="s">
+      <c r="A55" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="B55" s="22"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="23" t="s">
+      <c r="B55" s="30"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="F55" s="23"/>
-      <c r="G55" s="23"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
     </row>
     <row r="56" spans="1:7" ht="36" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
@@ -3810,17 +3814,17 @@
       <c r="G60" s="36"/>
     </row>
     <row r="61" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="22" t="s">
+      <c r="A61" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="22"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="23" t="s">
+      <c r="B61" s="30"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="F61" s="23"/>
-      <c r="G61" s="23"/>
+      <c r="F61" s="31"/>
+      <c r="G61" s="31"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
@@ -3892,17 +3896,17 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="22" t="s">
+      <c r="A65" s="30" t="s">
         <v>280</v>
       </c>
-      <c r="B65" s="22"/>
-      <c r="C65" s="22"/>
-      <c r="D65" s="22"/>
-      <c r="E65" s="23" t="s">
+      <c r="B65" s="30"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="31" t="s">
         <v>281</v>
       </c>
-      <c r="F65" s="23"/>
-      <c r="G65" s="23"/>
+      <c r="F65" s="31"/>
+      <c r="G65" s="31"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
@@ -3947,17 +3951,17 @@
       </c>
     </row>
     <row r="68" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="22" t="s">
+      <c r="A68" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="22"/>
-      <c r="E68" s="23" t="s">
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="F68" s="23"/>
-      <c r="G68" s="23"/>
+      <c r="F68" s="31"/>
+      <c r="G68" s="31"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="18" t="s">
@@ -3983,17 +3987,17 @@
       </c>
     </row>
     <row r="70" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="22" t="s">
+      <c r="A70" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="23" t="s">
+      <c r="B70" s="30"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="F70" s="23"/>
-      <c r="G70" s="23"/>
+      <c r="F70" s="31"/>
+      <c r="G70" s="31"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
@@ -4027,10 +4031,10 @@
       <c r="D72" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E72" s="29" t="s">
+      <c r="E72" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="F72" s="29" t="s">
+      <c r="F72" s="23" t="s">
         <v>205</v>
       </c>
       <c r="G72" s="16">
@@ -4112,17 +4116,17 @@
       <c r="G76" s="36"/>
     </row>
     <row r="77" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="22" t="s">
+      <c r="A77" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="B77" s="22"/>
-      <c r="C77" s="22"/>
-      <c r="D77" s="22"/>
-      <c r="E77" s="23" t="s">
+      <c r="B77" s="30"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="F77" s="23"/>
-      <c r="G77" s="23"/>
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
     </row>
     <row r="78" spans="1:7" ht="36" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
@@ -4135,13 +4139,13 @@
       <c r="D78" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="E78" s="29" t="s">
+      <c r="E78" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="F78" s="29" t="s">
+      <c r="F78" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="G78" s="29" t="s">
+      <c r="G78" s="23" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4156,13 +4160,13 @@
       <c r="D79" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="E79" s="29" t="s">
+      <c r="E79" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="F79" s="29" t="s">
+      <c r="F79" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="G79" s="29" t="s">
+      <c r="G79" s="23" t="s">
         <v>208</v>
       </c>
     </row>
@@ -4188,17 +4192,17 @@
       </c>
     </row>
     <row r="81" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="22" t="s">
+      <c r="A81" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="B81" s="22"/>
-      <c r="C81" s="22"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="23" t="s">
+      <c r="B81" s="30"/>
+      <c r="C81" s="30"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="F81" s="23"/>
-      <c r="G81" s="23"/>
+      <c r="F81" s="31"/>
+      <c r="G81" s="31"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
@@ -4243,17 +4247,17 @@
       </c>
     </row>
     <row r="84" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="22" t="s">
+      <c r="A84" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="B84" s="22"/>
-      <c r="C84" s="22"/>
-      <c r="D84" s="22"/>
-      <c r="E84" s="23" t="s">
+      <c r="B84" s="30"/>
+      <c r="C84" s="30"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="F84" s="23"/>
-      <c r="G84" s="23"/>
+      <c r="F84" s="31"/>
+      <c r="G84" s="31"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
@@ -4300,17 +4304,17 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="22" t="s">
+      <c r="A87" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B87" s="22"/>
-      <c r="C87" s="22"/>
-      <c r="D87" s="22"/>
-      <c r="E87" s="23" t="s">
+      <c r="B87" s="30"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="F87" s="23"/>
-      <c r="G87" s="23"/>
+      <c r="F87" s="31"/>
+      <c r="G87" s="31"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="18" t="s">
@@ -4334,17 +4338,17 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="22" t="s">
+      <c r="A89" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="B89" s="22"/>
-      <c r="C89" s="22"/>
-      <c r="D89" s="22"/>
-      <c r="E89" s="23" t="s">
+      <c r="B89" s="30"/>
+      <c r="C89" s="30"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="F89" s="23"/>
-      <c r="G89" s="23"/>
+      <c r="F89" s="31"/>
+      <c r="G89" s="31"/>
     </row>
     <row r="90" spans="1:7" ht="36" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
@@ -4433,17 +4437,17 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="22" t="s">
+      <c r="A94" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="B94" s="22"/>
-      <c r="C94" s="22"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="23" t="s">
+      <c r="B94" s="30"/>
+      <c r="C94" s="30"/>
+      <c r="D94" s="30"/>
+      <c r="E94" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="F94" s="23"/>
-      <c r="G94" s="23"/>
+      <c r="F94" s="31"/>
+      <c r="G94" s="31"/>
     </row>
     <row r="95" spans="1:7" ht="36" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
@@ -4488,17 +4492,17 @@
       </c>
     </row>
     <row r="97" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="22" t="s">
+      <c r="A97" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="B97" s="22"/>
-      <c r="C97" s="22"/>
-      <c r="D97" s="22"/>
-      <c r="E97" s="23" t="s">
+      <c r="B97" s="30"/>
+      <c r="C97" s="30"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="F97" s="23"/>
-      <c r="G97" s="23"/>
+      <c r="F97" s="31"/>
+      <c r="G97" s="31"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
@@ -4536,13 +4540,13 @@
       <c r="D99" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="E99" s="29" t="s">
+      <c r="E99" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="F99" s="29" t="s">
+      <c r="F99" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="G99" s="29" t="s">
+      <c r="G99" s="23" t="s">
         <v>226</v>
       </c>
     </row>
@@ -4559,13 +4563,13 @@
       <c r="D100" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="E100" s="29" t="s">
+      <c r="E100" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="F100" s="29" t="s">
+      <c r="F100" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="G100" s="29" t="s">
+      <c r="G100" s="23" t="s">
         <v>224</v>
       </c>
     </row>
@@ -4582,13 +4586,13 @@
       <c r="D101" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="E101" s="29" t="s">
+      <c r="E101" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="F101" s="29" t="s">
+      <c r="F101" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="G101" s="29" t="s">
+      <c r="G101" s="23" t="s">
         <v>225</v>
       </c>
     </row>
@@ -4599,17 +4603,17 @@
       <c r="B102" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C102" s="31">
+      <c r="C102" s="24">
         <v>17</v>
       </c>
       <c r="D102" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="E102" s="30" t="s">
+      <c r="E102" s="39" t="s">
         <v>227</v>
       </c>
-      <c r="F102" s="30"/>
-      <c r="G102" s="30"/>
+      <c r="F102" s="39"/>
+      <c r="G102" s="39"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
@@ -4618,17 +4622,17 @@
       <c r="B103" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C103" s="31">
+      <c r="C103" s="24">
         <v>50</v>
       </c>
       <c r="D103" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="E103" s="30" t="s">
+      <c r="E103" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="F103" s="30"/>
-      <c r="G103" s="30"/>
+      <c r="F103" s="39"/>
+      <c r="G103" s="39"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
@@ -4637,17 +4641,17 @@
       <c r="B104" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C104" s="31">
+      <c r="C104" s="24">
         <v>13</v>
       </c>
       <c r="D104" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="E104" s="32" t="s">
+      <c r="E104" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="F104" s="32"/>
-      <c r="G104" s="32"/>
+      <c r="F104" s="38"/>
+      <c r="G104" s="38"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
@@ -4694,17 +4698,17 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="22" t="s">
+      <c r="A107" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="B107" s="22"/>
-      <c r="C107" s="22"/>
-      <c r="D107" s="22"/>
-      <c r="E107" s="23" t="s">
+      <c r="B107" s="30"/>
+      <c r="C107" s="30"/>
+      <c r="D107" s="30"/>
+      <c r="E107" s="31" t="s">
         <v>240</v>
       </c>
-      <c r="F107" s="23"/>
-      <c r="G107" s="23"/>
+      <c r="F107" s="31"/>
+      <c r="G107" s="31"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
@@ -4749,17 +4753,17 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="22" t="s">
+      <c r="A110" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="B110" s="22"/>
-      <c r="C110" s="22"/>
-      <c r="D110" s="22"/>
-      <c r="E110" s="23" t="s">
+      <c r="B110" s="30"/>
+      <c r="C110" s="30"/>
+      <c r="D110" s="30"/>
+      <c r="E110" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="F110" s="23"/>
-      <c r="G110" s="23"/>
+      <c r="F110" s="31"/>
+      <c r="G110" s="31"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="18" t="s">
@@ -4785,17 +4789,17 @@
       </c>
     </row>
     <row r="112" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="22" t="s">
+      <c r="A112" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="B112" s="22"/>
-      <c r="C112" s="22"/>
-      <c r="D112" s="22"/>
-      <c r="E112" s="23" t="s">
+      <c r="B112" s="30"/>
+      <c r="C112" s="30"/>
+      <c r="D112" s="30"/>
+      <c r="E112" s="31" t="s">
         <v>272</v>
       </c>
-      <c r="F112" s="23"/>
-      <c r="G112" s="23"/>
+      <c r="F112" s="31"/>
+      <c r="G112" s="31"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="18" t="s">
@@ -4832,17 +4836,17 @@
       <c r="G114" s="36"/>
     </row>
     <row r="115" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="22" t="s">
+      <c r="A115" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="B115" s="22"/>
-      <c r="C115" s="22"/>
-      <c r="D115" s="22"/>
-      <c r="E115" s="23" t="s">
+      <c r="B115" s="30"/>
+      <c r="C115" s="30"/>
+      <c r="D115" s="30"/>
+      <c r="E115" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="F115" s="23"/>
-      <c r="G115" s="23"/>
+      <c r="F115" s="31"/>
+      <c r="G115" s="31"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
@@ -4857,13 +4861,13 @@
       <c r="D116" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="E116" s="33">
+      <c r="E116" s="37">
         <v>276800</v>
       </c>
-      <c r="F116" s="33">
+      <c r="F116" s="37">
         <v>167800</v>
       </c>
-      <c r="G116" s="33">
+      <c r="G116" s="37">
         <v>156000</v>
       </c>
     </row>
@@ -4878,20 +4882,20 @@
       <c r="D117" s="18" t="s">
         <v>310</v>
       </c>
-      <c r="E117" s="33"/>
-      <c r="F117" s="33"/>
-      <c r="G117" s="33"/>
+      <c r="E117" s="37"/>
+      <c r="F117" s="37"/>
+      <c r="G117" s="37"/>
     </row>
     <row r="118" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="34" t="s">
+      <c r="A118" s="32" t="s">
         <v>312</v>
       </c>
-      <c r="B118" s="24"/>
-      <c r="C118" s="24"/>
-      <c r="D118" s="24"/>
-      <c r="E118" s="24"/>
-      <c r="F118" s="24"/>
-      <c r="G118" s="24"/>
+      <c r="B118" s="28"/>
+      <c r="C118" s="28"/>
+      <c r="D118" s="28"/>
+      <c r="E118" s="28"/>
+      <c r="F118" s="28"/>
+      <c r="G118" s="28"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="18" t="s">
@@ -4906,17 +4910,17 @@
       </c>
     </row>
     <row r="120" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="22" t="s">
+      <c r="A120" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="B120" s="22"/>
-      <c r="C120" s="22"/>
-      <c r="D120" s="22"/>
-      <c r="E120" s="23" t="s">
+      <c r="B120" s="30"/>
+      <c r="C120" s="30"/>
+      <c r="D120" s="30"/>
+      <c r="E120" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="F120" s="23"/>
-      <c r="G120" s="23"/>
+      <c r="F120" s="31"/>
+      <c r="G120" s="31"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
@@ -4931,13 +4935,13 @@
       <c r="D121" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="E121" s="33">
+      <c r="E121" s="37">
         <v>256000</v>
       </c>
-      <c r="F121" s="33">
+      <c r="F121" s="37">
         <v>145540</v>
       </c>
-      <c r="G121" s="33">
+      <c r="G121" s="37">
         <v>125000</v>
       </c>
     </row>
@@ -4952,20 +4956,20 @@
       <c r="D122" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="E122" s="33"/>
-      <c r="F122" s="33"/>
-      <c r="G122" s="33"/>
+      <c r="E122" s="37"/>
+      <c r="F122" s="37"/>
+      <c r="G122" s="37"/>
     </row>
     <row r="123" spans="1:7" ht="70" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="34" t="s">
+      <c r="A123" s="32" t="s">
         <v>306</v>
       </c>
-      <c r="B123" s="24"/>
-      <c r="C123" s="24"/>
-      <c r="D123" s="24"/>
-      <c r="E123" s="24"/>
-      <c r="F123" s="24"/>
-      <c r="G123" s="24"/>
+      <c r="B123" s="28"/>
+      <c r="C123" s="28"/>
+      <c r="D123" s="28"/>
+      <c r="E123" s="28"/>
+      <c r="F123" s="28"/>
+      <c r="G123" s="28"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
@@ -4992,28 +4996,28 @@
       </c>
     </row>
     <row r="126" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="34" t="s">
+      <c r="A126" s="32" t="s">
         <v>347</v>
       </c>
-      <c r="B126" s="24"/>
-      <c r="C126" s="24"/>
-      <c r="D126" s="24"/>
-      <c r="E126" s="24"/>
-      <c r="F126" s="24"/>
-      <c r="G126" s="24"/>
+      <c r="B126" s="28"/>
+      <c r="C126" s="28"/>
+      <c r="D126" s="28"/>
+      <c r="E126" s="28"/>
+      <c r="F126" s="28"/>
+      <c r="G126" s="28"/>
     </row>
     <row r="127" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="22" t="s">
+      <c r="A127" s="30" t="s">
         <v>395</v>
       </c>
-      <c r="B127" s="22"/>
-      <c r="C127" s="22"/>
-      <c r="D127" s="22"/>
-      <c r="E127" s="23" t="s">
+      <c r="B127" s="30"/>
+      <c r="C127" s="30"/>
+      <c r="D127" s="30"/>
+      <c r="E127" s="31" t="s">
         <v>394</v>
       </c>
-      <c r="F127" s="23"/>
-      <c r="G127" s="23"/>
+      <c r="F127" s="31"/>
+      <c r="G127" s="31"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="18" t="s">
@@ -5039,17 +5043,17 @@
       </c>
     </row>
     <row r="129" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="22" t="s">
+      <c r="A129" s="30" t="s">
         <v>397</v>
       </c>
-      <c r="B129" s="22"/>
-      <c r="C129" s="22"/>
-      <c r="D129" s="22"/>
-      <c r="E129" s="23" t="s">
+      <c r="B129" s="30"/>
+      <c r="C129" s="30"/>
+      <c r="D129" s="30"/>
+      <c r="E129" s="31" t="s">
         <v>396</v>
       </c>
-      <c r="F129" s="23"/>
-      <c r="G129" s="23"/>
+      <c r="F129" s="31"/>
+      <c r="G129" s="31"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="18" t="s">
@@ -5075,17 +5079,17 @@
       </c>
     </row>
     <row r="131" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="22" t="s">
+      <c r="A131" s="30" t="s">
         <v>399</v>
       </c>
-      <c r="B131" s="22"/>
-      <c r="C131" s="22"/>
-      <c r="D131" s="22"/>
-      <c r="E131" s="23" t="s">
+      <c r="B131" s="30"/>
+      <c r="C131" s="30"/>
+      <c r="D131" s="30"/>
+      <c r="E131" s="31" t="s">
         <v>398</v>
       </c>
-      <c r="F131" s="23"/>
-      <c r="G131" s="23"/>
+      <c r="F131" s="31"/>
+      <c r="G131" s="31"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="18" t="s">
@@ -5111,52 +5115,52 @@
       </c>
     </row>
     <row r="133" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="22" t="s">
+      <c r="A133" s="30" t="s">
         <v>333</v>
       </c>
-      <c r="B133" s="22"/>
-      <c r="C133" s="22"/>
-      <c r="D133" s="22"/>
-      <c r="E133" s="23" t="s">
+      <c r="B133" s="30"/>
+      <c r="C133" s="30"/>
+      <c r="D133" s="30"/>
+      <c r="E133" s="31" t="s">
         <v>332</v>
       </c>
-      <c r="F133" s="23"/>
-      <c r="G133" s="23"/>
+      <c r="F133" s="31"/>
+      <c r="G133" s="31"/>
     </row>
     <row r="134" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="40" t="s">
+      <c r="A134" s="34" t="s">
         <v>349</v>
       </c>
-      <c r="B134" s="39"/>
-      <c r="C134" s="39"/>
-      <c r="D134" s="39"/>
-      <c r="E134" s="39"/>
-      <c r="F134" s="39"/>
-      <c r="G134" s="39"/>
-    </row>
-    <row r="135" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="38" t="s">
+      <c r="B134" s="35"/>
+      <c r="C134" s="35"/>
+      <c r="D134" s="35"/>
+      <c r="E134" s="35"/>
+      <c r="F134" s="35"/>
+      <c r="G134" s="35"/>
+    </row>
+    <row r="135" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="33" t="s">
         <v>416</v>
       </c>
-      <c r="B135" s="38"/>
-      <c r="C135" s="38"/>
-      <c r="D135" s="38"/>
-      <c r="E135" s="44" t="s">
+      <c r="B135" s="33"/>
+      <c r="C135" s="33"/>
+      <c r="D135" s="33"/>
+      <c r="E135" s="29" t="s">
         <v>415</v>
       </c>
-      <c r="F135" s="44"/>
-      <c r="G135" s="44"/>
-    </row>
-    <row r="136" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="24" t="s">
+      <c r="F135" s="29"/>
+      <c r="G135" s="29"/>
+    </row>
+    <row r="136" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="28" t="s">
         <v>422</v>
       </c>
-      <c r="B136" s="24"/>
-      <c r="C136" s="24"/>
-      <c r="D136" s="24"/>
-      <c r="E136" s="24"/>
-      <c r="F136" s="24"/>
-      <c r="G136" s="24"/>
+      <c r="B136" s="28"/>
+      <c r="C136" s="28"/>
+      <c r="D136" s="28"/>
+      <c r="E136" s="28"/>
+      <c r="F136" s="28"/>
+      <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
@@ -5179,29 +5183,29 @@
         <v>437</v>
       </c>
     </row>
-    <row r="138" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="38" t="s">
+    <row r="138" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="33" t="s">
         <v>414</v>
       </c>
-      <c r="B138" s="38"/>
-      <c r="C138" s="38"/>
-      <c r="D138" s="38"/>
-      <c r="E138" s="44" t="s">
+      <c r="B138" s="33"/>
+      <c r="C138" s="33"/>
+      <c r="D138" s="33"/>
+      <c r="E138" s="29" t="s">
         <v>415</v>
       </c>
-      <c r="F138" s="44"/>
-      <c r="G138" s="44"/>
-    </row>
-    <row r="139" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="24" t="s">
+      <c r="F138" s="29"/>
+      <c r="G138" s="29"/>
+    </row>
+    <row r="139" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="28" t="s">
         <v>423</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
-      <c r="D139" s="24"/>
-      <c r="E139" s="24"/>
-      <c r="F139" s="24"/>
-      <c r="G139" s="24"/>
+      <c r="B139" s="28"/>
+      <c r="C139" s="28"/>
+      <c r="D139" s="28"/>
+      <c r="E139" s="28"/>
+      <c r="F139" s="28"/>
+      <c r="G139" s="28"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
@@ -5224,31 +5228,31 @@
         <v>438</v>
       </c>
     </row>
-    <row r="141" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="38" t="s">
+    <row r="141" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="33" t="s">
         <v>431</v>
       </c>
-      <c r="B141" s="38"/>
-      <c r="C141" s="38"/>
-      <c r="D141" s="38"/>
-      <c r="E141" s="46" t="s">
+      <c r="B141" s="33"/>
+      <c r="C141" s="33"/>
+      <c r="D141" s="33"/>
+      <c r="E141" s="27" t="s">
         <v>428</v>
       </c>
-      <c r="F141" s="44" t="s">
+      <c r="F141" s="29" t="s">
         <v>429</v>
       </c>
-      <c r="G141" s="44"/>
-    </row>
-    <row r="142" spans="1:7" s="37" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="34" t="s">
+      <c r="G141" s="29"/>
+    </row>
+    <row r="142" spans="1:7" s="25" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="32" t="s">
         <v>430</v>
       </c>
-      <c r="B142" s="24"/>
-      <c r="C142" s="24"/>
-      <c r="D142" s="24"/>
-      <c r="E142" s="24"/>
-      <c r="F142" s="24"/>
-      <c r="G142" s="24"/>
+      <c r="B142" s="28"/>
+      <c r="C142" s="28"/>
+      <c r="D142" s="28"/>
+      <c r="E142" s="28"/>
+      <c r="F142" s="28"/>
+      <c r="G142" s="28"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
@@ -5267,33 +5271,33 @@
       <c r="F143" s="1">
         <v>60000</v>
       </c>
-      <c r="G143" s="29">
+      <c r="G143" s="23">
         <v>45000</v>
       </c>
     </row>
-    <row r="144" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="38" t="s">
+    <row r="144" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="33" t="s">
         <v>350</v>
       </c>
-      <c r="B144" s="38"/>
-      <c r="C144" s="38"/>
-      <c r="D144" s="38"/>
-      <c r="E144" s="44" t="s">
+      <c r="B144" s="33"/>
+      <c r="C144" s="33"/>
+      <c r="D144" s="33"/>
+      <c r="E144" s="29" t="s">
         <v>350</v>
       </c>
-      <c r="F144" s="44"/>
-      <c r="G144" s="44"/>
-    </row>
-    <row r="145" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="24" t="s">
+      <c r="F144" s="29"/>
+      <c r="G144" s="29"/>
+    </row>
+    <row r="145" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="28" t="s">
         <v>424</v>
       </c>
-      <c r="B145" s="24"/>
-      <c r="C145" s="24"/>
-      <c r="D145" s="24"/>
-      <c r="E145" s="24"/>
-      <c r="F145" s="24"/>
-      <c r="G145" s="24"/>
+      <c r="B145" s="28"/>
+      <c r="C145" s="28"/>
+      <c r="D145" s="28"/>
+      <c r="E145" s="28"/>
+      <c r="F145" s="28"/>
+      <c r="G145" s="28"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
@@ -5312,37 +5316,37 @@
       <c r="F146" s="1">
         <v>5000</v>
       </c>
-      <c r="G146" s="29">
+      <c r="G146" s="23">
         <v>5000</v>
       </c>
     </row>
-    <row r="147" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="38" t="s">
+    <row r="147" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="33" t="s">
         <v>421</v>
       </c>
-      <c r="B147" s="38"/>
-      <c r="C147" s="38"/>
-      <c r="D147" s="38"/>
-      <c r="E147" s="46" t="s">
+      <c r="B147" s="33"/>
+      <c r="C147" s="33"/>
+      <c r="D147" s="33"/>
+      <c r="E147" s="27" t="s">
         <v>417</v>
       </c>
-      <c r="F147" s="46" t="s">
+      <c r="F147" s="27" t="s">
         <v>432</v>
       </c>
-      <c r="G147" s="46" t="s">
+      <c r="G147" s="27" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="148" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="24" t="s">
+    <row r="148" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="28" t="s">
         <v>425</v>
       </c>
-      <c r="B148" s="24"/>
-      <c r="C148" s="24"/>
-      <c r="D148" s="24"/>
-      <c r="E148" s="24"/>
-      <c r="F148" s="24"/>
-      <c r="G148" s="24"/>
+      <c r="B148" s="28"/>
+      <c r="C148" s="28"/>
+      <c r="D148" s="28"/>
+      <c r="E148" s="28"/>
+      <c r="F148" s="28"/>
+      <c r="G148" s="28"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
@@ -5365,40 +5369,67 @@
         <v>439</v>
       </c>
     </row>
-    <row r="150" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="150" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C151" s="1"/>
     </row>
-    <row r="152" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C153" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="91">
-    <mergeCell ref="A148:G148"/>
-    <mergeCell ref="F141:G141"/>
-    <mergeCell ref="A127:D127"/>
-    <mergeCell ref="E127:G127"/>
-    <mergeCell ref="A129:D129"/>
-    <mergeCell ref="E129:G129"/>
-    <mergeCell ref="A131:D131"/>
-    <mergeCell ref="E131:G131"/>
-    <mergeCell ref="A136:G136"/>
-    <mergeCell ref="A139:G139"/>
-    <mergeCell ref="A142:G142"/>
-    <mergeCell ref="A145:G145"/>
-    <mergeCell ref="A147:D147"/>
-    <mergeCell ref="A126:G126"/>
-    <mergeCell ref="A134:G134"/>
-    <mergeCell ref="A138:D138"/>
-    <mergeCell ref="E138:G138"/>
-    <mergeCell ref="A141:D141"/>
-    <mergeCell ref="A144:D144"/>
-    <mergeCell ref="E144:G144"/>
-    <mergeCell ref="A133:D133"/>
-    <mergeCell ref="E133:G133"/>
-    <mergeCell ref="A135:D135"/>
-    <mergeCell ref="E135:G135"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="E84:G84"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E104:G104"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="E97:G97"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="E102:G102"/>
+    <mergeCell ref="E103:G103"/>
+    <mergeCell ref="A97:D97"/>
+    <mergeCell ref="A94:D94"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="E89:G89"/>
+    <mergeCell ref="E94:G94"/>
+    <mergeCell ref="F116:F117"/>
+    <mergeCell ref="G116:G117"/>
+    <mergeCell ref="E107:G107"/>
+    <mergeCell ref="A110:D110"/>
+    <mergeCell ref="E110:G110"/>
     <mergeCell ref="A123:G123"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A60:G60"/>
@@ -5415,57 +5446,30 @@
     <mergeCell ref="A115:D115"/>
     <mergeCell ref="E115:G115"/>
     <mergeCell ref="E116:E117"/>
-    <mergeCell ref="F116:F117"/>
-    <mergeCell ref="G116:G117"/>
-    <mergeCell ref="E107:G107"/>
-    <mergeCell ref="A110:D110"/>
-    <mergeCell ref="E110:G110"/>
-    <mergeCell ref="E104:G104"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="E97:G97"/>
-    <mergeCell ref="A87:D87"/>
-    <mergeCell ref="E87:G87"/>
-    <mergeCell ref="E102:G102"/>
-    <mergeCell ref="E103:G103"/>
-    <mergeCell ref="A97:D97"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A94:D94"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="E81:G81"/>
-    <mergeCell ref="E84:G84"/>
-    <mergeCell ref="E89:G89"/>
-    <mergeCell ref="E94:G94"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="A126:G126"/>
+    <mergeCell ref="A134:G134"/>
+    <mergeCell ref="A138:D138"/>
+    <mergeCell ref="E138:G138"/>
+    <mergeCell ref="A141:D141"/>
+    <mergeCell ref="A133:D133"/>
+    <mergeCell ref="E133:G133"/>
+    <mergeCell ref="A135:D135"/>
+    <mergeCell ref="E135:G135"/>
+    <mergeCell ref="A148:G148"/>
+    <mergeCell ref="F141:G141"/>
+    <mergeCell ref="A127:D127"/>
+    <mergeCell ref="E127:G127"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="E129:G129"/>
+    <mergeCell ref="A131:D131"/>
+    <mergeCell ref="E131:G131"/>
+    <mergeCell ref="A136:G136"/>
+    <mergeCell ref="A139:G139"/>
+    <mergeCell ref="A142:G142"/>
+    <mergeCell ref="A145:G145"/>
+    <mergeCell ref="A147:D147"/>
+    <mergeCell ref="A144:D144"/>
+    <mergeCell ref="E144:G144"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5475,10 +5479,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D22479B-6493-4CBB-9E78-1BDB1D2E35D0}">
-  <dimension ref="A1:G117"/>
+  <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -5487,77 +5491,77 @@
     <col min="2" max="2" width="10.58203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.58203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="50.58203125" style="1" customWidth="1"/>
-    <col min="5" max="7" width="20.58203125" style="29" customWidth="1"/>
+    <col min="5" max="7" width="20.58203125" style="23" customWidth="1"/>
     <col min="8" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="41" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="44" t="s">
         <v>267</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="28" t="s">
         <v>351</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="45" t="s">
         <v>391</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="44" t="s">
         <v>284</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -5572,13 +5576,13 @@
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="26" t="s">
         <v>200</v>
       </c>
     </row>
@@ -5594,12 +5598,12 @@
       <c r="G8" s="36"/>
     </row>
     <row r="9" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="43" t="s">
         <v>40</v>
       </c>
@@ -5617,26 +5621,26 @@
       <c r="D10" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="23">
         <v>31</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="23">
         <v>29</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="23">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -5649,23 +5653,23 @@
       <c r="D12" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="23">
         <v>2</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="23">
         <v>3</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="23">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="43" t="s">
         <v>41</v>
       </c>
@@ -5683,26 +5687,26 @@
       <c r="D14" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="23">
         <v>65</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="23" t="s">
         <v>353</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="23" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -5715,23 +5719,23 @@
       <c r="D16" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="23" t="s">
         <v>361</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="23" t="s">
         <v>362</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="23" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="43" t="s">
         <v>56</v>
       </c>
@@ -5749,26 +5753,26 @@
       <c r="D18" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="23" t="s">
         <v>356</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="23" t="s">
         <v>356</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="G18" s="23" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -5781,23 +5785,23 @@
       <c r="D20" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="23" t="s">
         <v>354</v>
       </c>
-      <c r="G20" s="29" t="s">
+      <c r="G20" s="23" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="43" t="s">
         <v>67</v>
       </c>
@@ -5815,26 +5819,26 @@
       <c r="D22" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="23" t="s">
         <v>363</v>
       </c>
-      <c r="F22" s="29" t="s">
+      <c r="F22" s="23" t="s">
         <v>364</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="G22" s="23" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -5847,23 +5851,23 @@
       <c r="D24" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="F24" s="29" t="s">
+      <c r="F24" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="23" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
       <c r="E25" s="43" t="s">
         <v>85</v>
       </c>
@@ -5881,13 +5885,13 @@
       <c r="D26" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="23" t="s">
         <v>367</v>
       </c>
-      <c r="F26" s="29" t="s">
+      <c r="F26" s="23" t="s">
         <v>368</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="23" t="s">
         <v>369</v>
       </c>
     </row>
@@ -5902,23 +5906,23 @@
       <c r="D27" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E27" s="29" t="s">
+      <c r="E27" s="23" t="s">
         <v>370</v>
       </c>
-      <c r="F27" s="29" t="s">
+      <c r="F27" s="23" t="s">
         <v>371</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G27" s="23" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
       <c r="E28" s="43" t="s">
         <v>113</v>
       </c>
@@ -5936,13 +5940,13 @@
       <c r="D29" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E29" s="29" t="s">
+      <c r="E29" s="23" t="s">
         <v>372</v>
       </c>
-      <c r="F29" s="29" t="s">
+      <c r="F29" s="23" t="s">
         <v>373</v>
       </c>
-      <c r="G29" s="29" t="s">
+      <c r="G29" s="23" t="s">
         <v>374</v>
       </c>
     </row>
@@ -5957,13 +5961,13 @@
       <c r="D30" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E30" s="29" t="s">
+      <c r="E30" s="23" t="s">
         <v>375</v>
       </c>
-      <c r="F30" s="29" t="s">
+      <c r="F30" s="23" t="s">
         <v>371</v>
       </c>
-      <c r="G30" s="29" t="s">
+      <c r="G30" s="23" t="s">
         <v>371</v>
       </c>
     </row>
@@ -5979,12 +5983,12 @@
       <c r="G31" s="36"/>
     </row>
     <row r="32" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
       <c r="E32" s="43" t="s">
         <v>119</v>
       </c>
@@ -6002,13 +6006,13 @@
       <c r="D33" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E33" s="29" t="s">
+      <c r="E33" s="23" t="s">
         <v>376</v>
       </c>
-      <c r="F33" s="29" t="s">
+      <c r="F33" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="G33" s="29" t="s">
+      <c r="G33" s="23" t="s">
         <v>382</v>
       </c>
     </row>
@@ -6023,34 +6027,34 @@
       <c r="D34" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E34" s="29" t="s">
+      <c r="E34" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="F34" s="29" t="s">
+      <c r="F34" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G34" s="29" t="s">
+      <c r="G34" s="23" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="32" t="s">
         <v>277</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
     </row>
     <row r="36" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="22" t="s">
+      <c r="A36" s="30" t="s">
         <v>280</v>
       </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
       <c r="E36" s="43" t="s">
         <v>281</v>
       </c>
@@ -6068,13 +6072,13 @@
       <c r="D37" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E37" s="29" t="s">
+      <c r="E37" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="F37" s="29" t="s">
+      <c r="F37" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="G37" s="29" t="s">
+      <c r="G37" s="23" t="s">
         <v>378</v>
       </c>
     </row>
@@ -6089,23 +6093,23 @@
       <c r="D38" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E38" s="29" t="s">
+      <c r="E38" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="F38" s="29" t="s">
+      <c r="F38" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="G38" s="29" t="s">
+      <c r="G38" s="23" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
       <c r="E39" s="43" t="s">
         <v>122</v>
       </c>
@@ -6123,13 +6127,13 @@
       <c r="D40" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E40" s="29" t="s">
+      <c r="E40" s="23" t="s">
         <v>376</v>
       </c>
-      <c r="F40" s="29" t="s">
+      <c r="F40" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="G40" s="29" t="s">
+      <c r="G40" s="23" t="s">
         <v>382</v>
       </c>
     </row>
@@ -6144,23 +6148,23 @@
       <c r="D41" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E41" s="29" t="s">
+      <c r="E41" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="F41" s="29" t="s">
+      <c r="F41" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G41" s="29" t="s">
+      <c r="G41" s="23" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
       <c r="E42" s="43" t="s">
         <v>125</v>
       </c>
@@ -6178,13 +6182,13 @@
       <c r="D43" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E43" s="29" t="s">
+      <c r="E43" s="23" t="s">
         <v>365</v>
       </c>
-      <c r="F43" s="29" t="s">
+      <c r="F43" s="23" t="s">
         <v>363</v>
       </c>
-      <c r="G43" s="29" t="s">
+      <c r="G43" s="23" t="s">
         <v>365</v>
       </c>
     </row>
@@ -6199,13 +6203,13 @@
       <c r="D44" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E44" s="29" t="s">
+      <c r="E44" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="F44" s="29" t="s">
+      <c r="F44" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G44" s="29" t="s">
+      <c r="G44" s="23" t="s">
         <v>358</v>
       </c>
     </row>
@@ -6221,12 +6225,12 @@
       <c r="G45" s="36"/>
     </row>
     <row r="46" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
       <c r="E46" s="43" t="s">
         <v>139</v>
       </c>
@@ -6244,13 +6248,13 @@
       <c r="D47" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E47" s="29" t="s">
+      <c r="E47" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="F47" s="29" t="s">
+      <c r="F47" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="G47" s="29" t="s">
+      <c r="G47" s="23" t="s">
         <v>365</v>
       </c>
     </row>
@@ -6265,34 +6269,34 @@
       <c r="D48" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E48" s="29" t="s">
+      <c r="E48" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="F48" s="29" t="s">
+      <c r="F48" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G48" s="29" t="s">
+      <c r="G48" s="23" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="28" t="s">
         <v>291</v>
       </c>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
     </row>
     <row r="50" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="22" t="s">
+      <c r="A50" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
       <c r="E50" s="43" t="s">
         <v>156</v>
       </c>
@@ -6310,13 +6314,13 @@
       <c r="D51" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E51" s="29" t="s">
+      <c r="E51" s="23" t="s">
         <v>386</v>
       </c>
-      <c r="F51" s="29" t="s">
+      <c r="F51" s="23" t="s">
         <v>386</v>
       </c>
-      <c r="G51" s="29" t="s">
+      <c r="G51" s="23" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6331,23 +6335,23 @@
       <c r="D52" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E52" s="29" t="s">
+      <c r="E52" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="F52" s="29" t="s">
+      <c r="F52" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="G52" s="29" t="s">
+      <c r="G52" s="23" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="22" t="s">
+      <c r="A53" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="B53" s="22"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
       <c r="E53" s="43" t="s">
         <v>210</v>
       </c>
@@ -6365,13 +6369,13 @@
       <c r="D54" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E54" s="29" t="s">
+      <c r="E54" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="F54" s="29" t="s">
+      <c r="F54" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="G54" s="29" t="s">
+      <c r="G54" s="23" t="s">
         <v>381</v>
       </c>
     </row>
@@ -6386,23 +6390,23 @@
       <c r="D55" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E55" s="29" t="s">
+      <c r="E55" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="F55" s="29" t="s">
+      <c r="F55" s="23" t="s">
         <v>392</v>
       </c>
-      <c r="G55" s="29" t="s">
+      <c r="G55" s="23" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="22" t="s">
+      <c r="A56" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B56" s="22"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="22"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
       <c r="E56" s="43" t="s">
         <v>213</v>
       </c>
@@ -6420,13 +6424,13 @@
       <c r="D57" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E57" s="29" t="s">
+      <c r="E57" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="F57" s="29" t="s">
+      <c r="F57" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="G57" s="29" t="s">
+      <c r="G57" s="23" t="s">
         <v>365</v>
       </c>
     </row>
@@ -6441,23 +6445,23 @@
       <c r="D58" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E58" s="29" t="s">
+      <c r="E58" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="F58" s="29" t="s">
+      <c r="F58" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G58" s="29" t="s">
+      <c r="G58" s="23" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="22" t="s">
+      <c r="A59" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="B59" s="22"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
       <c r="E59" s="43" t="s">
         <v>170</v>
       </c>
@@ -6475,13 +6479,13 @@
       <c r="D60" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E60" s="29" t="s">
+      <c r="E60" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="F60" s="29" t="s">
+      <c r="F60" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="G60" s="29" t="s">
+      <c r="G60" s="23" t="s">
         <v>369</v>
       </c>
     </row>
@@ -6496,23 +6500,23 @@
       <c r="D61" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E61" s="29" t="s">
+      <c r="E61" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="F61" s="29" t="s">
+      <c r="F61" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G61" s="29" t="s">
+      <c r="G61" s="23" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="22" t="s">
+      <c r="A62" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="B62" s="22"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="22"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="30"/>
       <c r="E62" s="43" t="s">
         <v>172</v>
       </c>
@@ -6530,13 +6534,13 @@
       <c r="D63" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E63" s="29" t="s">
+      <c r="E63" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="F63" s="29" t="s">
+      <c r="F63" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="G63" s="29" t="s">
+      <c r="G63" s="23" t="s">
         <v>381</v>
       </c>
     </row>
@@ -6551,23 +6555,23 @@
       <c r="D64" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E64" s="29" t="s">
+      <c r="E64" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="F64" s="29" t="s">
+      <c r="F64" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="G64" s="29" t="s">
+      <c r="G64" s="23" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="22" t="s">
+      <c r="A65" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="B65" s="22"/>
-      <c r="C65" s="22"/>
-      <c r="D65" s="22"/>
+      <c r="B65" s="30"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="30"/>
       <c r="E65" s="43" t="s">
         <v>271</v>
       </c>
@@ -6585,13 +6589,13 @@
       <c r="D66" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E66" s="29" t="s">
+      <c r="E66" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="F66" s="29" t="s">
+      <c r="F66" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="G66" s="29" t="s">
+      <c r="G66" s="23" t="s">
         <v>365</v>
       </c>
     </row>
@@ -6606,23 +6610,23 @@
       <c r="D67" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E67" s="29" t="s">
+      <c r="E67" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="F67" s="29" t="s">
+      <c r="F67" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G67" s="29" t="s">
+      <c r="G67" s="23" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="22" t="s">
+      <c r="A68" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="22"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
       <c r="E68" s="43" t="s">
         <v>240</v>
       </c>
@@ -6640,13 +6644,13 @@
       <c r="D69" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E69" s="29" t="s">
+      <c r="E69" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="F69" s="29" t="s">
+      <c r="F69" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="G69" s="29" t="s">
+      <c r="G69" s="23" t="s">
         <v>365</v>
       </c>
     </row>
@@ -6661,23 +6665,23 @@
       <c r="D70" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E70" s="29" t="s">
+      <c r="E70" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="F70" s="29" t="s">
+      <c r="F70" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="G70" s="29" t="s">
+      <c r="G70" s="23" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="22" t="s">
+      <c r="A71" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="B71" s="22"/>
-      <c r="C71" s="22"/>
-      <c r="D71" s="22"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
       <c r="E71" s="43" t="s">
         <v>239</v>
       </c>
@@ -6695,13 +6699,13 @@
       <c r="D72" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E72" s="29" t="s">
+      <c r="E72" s="23" t="s">
         <v>367</v>
       </c>
-      <c r="F72" s="29" t="s">
+      <c r="F72" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="G72" s="29" t="s">
+      <c r="G72" s="23" t="s">
         <v>369</v>
       </c>
     </row>
@@ -6716,23 +6720,23 @@
       <c r="D73" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E73" s="29" t="s">
+      <c r="E73" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="F73" s="29" t="s">
+      <c r="F73" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G73" s="29" t="s">
+      <c r="G73" s="23" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="22" t="s">
+      <c r="A74" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="B74" s="22"/>
-      <c r="C74" s="22"/>
-      <c r="D74" s="22"/>
+      <c r="B74" s="30"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="30"/>
       <c r="E74" s="43" t="s">
         <v>272</v>
       </c>
@@ -6750,13 +6754,13 @@
       <c r="D75" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E75" s="29" t="s">
+      <c r="E75" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F75" s="29" t="s">
+      <c r="F75" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G75" s="29" t="s">
+      <c r="G75" s="23" t="s">
         <v>10</v>
       </c>
     </row>
@@ -6771,26 +6775,26 @@
       <c r="D76" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E76" s="29" t="s">
+      <c r="E76" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F76" s="29" t="s">
+      <c r="F76" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G76" s="29" t="s">
+      <c r="G76" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="24" t="s">
+      <c r="A77" s="28" t="s">
         <v>393</v>
       </c>
-      <c r="B77" s="24"/>
-      <c r="C77" s="24"/>
-      <c r="D77" s="24"/>
-      <c r="E77" s="24"/>
-      <c r="F77" s="24"/>
-      <c r="G77" s="24"/>
+      <c r="B77" s="28"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="28"/>
+      <c r="F77" s="28"/>
+      <c r="G77" s="28"/>
     </row>
     <row r="78" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="36" t="s">
@@ -6804,12 +6808,12 @@
       <c r="G78" s="36"/>
     </row>
     <row r="79" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="22" t="s">
+      <c r="A79" s="30" t="s">
         <v>410</v>
       </c>
-      <c r="B79" s="22"/>
-      <c r="C79" s="22"/>
-      <c r="D79" s="22"/>
+      <c r="B79" s="30"/>
+      <c r="C79" s="30"/>
+      <c r="D79" s="30"/>
       <c r="E79" s="43" t="s">
         <v>409</v>
       </c>
@@ -6827,13 +6831,13 @@
       <c r="D80" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E80" s="29" t="s">
+      <c r="E80" s="23" t="s">
         <v>365</v>
       </c>
-      <c r="F80" s="29" t="s">
+      <c r="F80" s="23" t="s">
         <v>365</v>
       </c>
-      <c r="G80" s="29" t="s">
+      <c r="G80" s="23" t="s">
         <v>385</v>
       </c>
     </row>
@@ -6848,52 +6852,52 @@
       <c r="D81" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E81" s="29" t="s">
+      <c r="E81" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="F81" s="29" t="s">
+      <c r="F81" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G81" s="29" t="s">
+      <c r="G81" s="23" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="22" t="s">
+      <c r="A82" s="30" t="s">
         <v>333</v>
       </c>
-      <c r="B82" s="22"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="22"/>
+      <c r="B82" s="30"/>
+      <c r="C82" s="30"/>
+      <c r="D82" s="30"/>
       <c r="E82" s="43" t="s">
         <v>332</v>
       </c>
       <c r="F82" s="43"/>
       <c r="G82" s="43"/>
     </row>
-    <row r="83" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="38" t="s">
+    <row r="83" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="33" t="s">
         <v>416</v>
       </c>
-      <c r="B83" s="38"/>
-      <c r="C83" s="38"/>
-      <c r="D83" s="38"/>
-      <c r="E83" s="44" t="s">
+      <c r="B83" s="33"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="33"/>
+      <c r="E83" s="29" t="s">
         <v>415</v>
       </c>
-      <c r="F83" s="44"/>
-      <c r="G83" s="44"/>
+      <c r="F83" s="29"/>
+      <c r="G83" s="29"/>
     </row>
     <row r="84" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="24" t="s">
+      <c r="A84" s="28" t="s">
         <v>422</v>
       </c>
-      <c r="B84" s="24"/>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24"/>
-      <c r="G84" s="24"/>
+      <c r="B84" s="28"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="28"/>
+      <c r="F84" s="28"/>
+      <c r="G84" s="28"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
@@ -6906,13 +6910,13 @@
       <c r="D85" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E85" s="29" t="s">
+      <c r="E85" s="23" t="s">
         <v>367</v>
       </c>
-      <c r="F85" s="29" t="s">
+      <c r="F85" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="G85" s="29" t="s">
+      <c r="G85" s="23" t="s">
         <v>368</v>
       </c>
     </row>
@@ -6927,39 +6931,39 @@
       <c r="D86" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E86" s="29" t="s">
+      <c r="E86" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="F86" s="29" t="s">
+      <c r="F86" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G86" s="29" t="s">
+      <c r="G86" s="23" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="38" t="s">
+    <row r="87" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="33" t="s">
         <v>414</v>
       </c>
-      <c r="B87" s="38"/>
-      <c r="C87" s="38"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="44" t="s">
+      <c r="B87" s="33"/>
+      <c r="C87" s="33"/>
+      <c r="D87" s="33"/>
+      <c r="E87" s="29" t="s">
         <v>415</v>
       </c>
-      <c r="F87" s="44"/>
-      <c r="G87" s="44"/>
-    </row>
-    <row r="88" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="24" t="s">
+      <c r="F87" s="29"/>
+      <c r="G87" s="29"/>
+    </row>
+    <row r="88" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="28" t="s">
         <v>423</v>
       </c>
-      <c r="B88" s="24"/>
-      <c r="C88" s="24"/>
-      <c r="D88" s="24"/>
-      <c r="E88" s="24"/>
-      <c r="F88" s="24"/>
-      <c r="G88" s="24"/>
+      <c r="B88" s="28"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="28"/>
+      <c r="F88" s="28"/>
+      <c r="G88" s="28"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
@@ -6972,13 +6976,13 @@
       <c r="D89" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E89" s="29" t="s">
+      <c r="E89" s="23" t="s">
         <v>413</v>
       </c>
-      <c r="F89" s="29" t="s">
+      <c r="F89" s="23" t="s">
         <v>435</v>
       </c>
-      <c r="G89" s="29" t="s">
+      <c r="G89" s="23" t="s">
         <v>367</v>
       </c>
     </row>
@@ -6993,41 +6997,41 @@
       <c r="D90" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E90" s="29" t="s">
+      <c r="E90" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="F90" s="29" t="s">
+      <c r="F90" s="23" t="s">
         <v>435</v>
       </c>
-      <c r="G90" s="29" t="s">
+      <c r="G90" s="23" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="91" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="38" t="s">
+    <row r="91" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="33" t="s">
         <v>431</v>
       </c>
-      <c r="B91" s="38"/>
-      <c r="C91" s="38"/>
-      <c r="D91" s="38"/>
-      <c r="E91" s="46" t="s">
+      <c r="B91" s="33"/>
+      <c r="C91" s="33"/>
+      <c r="D91" s="33"/>
+      <c r="E91" s="27" t="s">
         <v>428</v>
       </c>
-      <c r="F91" s="44" t="s">
+      <c r="F91" s="29" t="s">
         <v>429</v>
       </c>
-      <c r="G91" s="44"/>
-    </row>
-    <row r="92" spans="1:7" s="37" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="34" t="s">
+      <c r="G91" s="29"/>
+    </row>
+    <row r="92" spans="1:7" s="25" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="32" t="s">
         <v>430</v>
       </c>
-      <c r="B92" s="24"/>
-      <c r="C92" s="24"/>
-      <c r="D92" s="24"/>
-      <c r="E92" s="24"/>
-      <c r="F92" s="24"/>
-      <c r="G92" s="24"/>
+      <c r="B92" s="28"/>
+      <c r="C92" s="28"/>
+      <c r="D92" s="28"/>
+      <c r="E92" s="28"/>
+      <c r="F92" s="28"/>
+      <c r="G92" s="28"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
@@ -7040,13 +7044,13 @@
       <c r="D93" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E93" s="29" t="s">
+      <c r="E93" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="F93" s="29" t="s">
+      <c r="F93" s="23" t="s">
         <v>368</v>
       </c>
-      <c r="G93" s="29" t="s">
+      <c r="G93" s="23" t="s">
         <v>413</v>
       </c>
     </row>
@@ -7061,41 +7065,41 @@
       <c r="D94" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E94" s="29" t="s">
+      <c r="E94" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="F94" s="29" t="s">
+      <c r="F94" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="G94" s="29" t="s">
+      <c r="G94" s="23" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="38" t="s">
+    <row r="95" spans="1:7" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="33" t="s">
         <v>350</v>
       </c>
-      <c r="B95" s="38"/>
-      <c r="C95" s="38"/>
-      <c r="D95" s="38"/>
-      <c r="E95" s="44" t="s">
+      <c r="B95" s="33"/>
+      <c r="C95" s="33"/>
+      <c r="D95" s="33"/>
+      <c r="E95" s="29" t="s">
         <v>350</v>
       </c>
-      <c r="F95" s="44"/>
-      <c r="G95" s="44"/>
-    </row>
-    <row r="96" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="24" t="s">
+      <c r="F95" s="29"/>
+      <c r="G95" s="29"/>
+    </row>
+    <row r="96" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="28" t="s">
         <v>424</v>
       </c>
-      <c r="B96" s="24"/>
-      <c r="C96" s="24"/>
-      <c r="D96" s="24"/>
-      <c r="E96" s="24"/>
-      <c r="F96" s="24"/>
-      <c r="G96" s="24"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B96" s="28"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="28"/>
+      <c r="F96" s="28"/>
+      <c r="G96" s="28"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>330</v>
       </c>
@@ -7106,17 +7110,17 @@
       <c r="D97" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E97" s="29" t="s">
+      <c r="E97" s="23" t="s">
         <v>426</v>
       </c>
-      <c r="F97" s="29" t="s">
+      <c r="F97" s="23" t="s">
         <v>436</v>
       </c>
-      <c r="G97" s="29" t="s">
+      <c r="G97" s="23" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>331</v>
       </c>
@@ -7127,45 +7131,45 @@
       <c r="D98" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E98" s="29" t="s">
+      <c r="E98" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="F98" s="29" t="s">
+      <c r="F98" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="G98" s="29" t="s">
+      <c r="G98" s="23" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="99" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="38" t="s">
+    <row r="99" spans="1:8" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="33" t="s">
         <v>421</v>
       </c>
-      <c r="B99" s="38"/>
-      <c r="C99" s="38"/>
-      <c r="D99" s="38"/>
-      <c r="E99" s="46" t="s">
+      <c r="B99" s="33"/>
+      <c r="C99" s="33"/>
+      <c r="D99" s="33"/>
+      <c r="E99" s="27" t="s">
         <v>417</v>
       </c>
-      <c r="F99" s="46" t="s">
+      <c r="F99" s="27" t="s">
         <v>432</v>
       </c>
-      <c r="G99" s="46" t="s">
+      <c r="G99" s="27" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="100" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="24" t="s">
+    <row r="100" spans="1:8" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="28" t="s">
         <v>425</v>
       </c>
-      <c r="B100" s="24"/>
-      <c r="C100" s="24"/>
-      <c r="D100" s="24"/>
-      <c r="E100" s="24"/>
-      <c r="F100" s="24"/>
-      <c r="G100" s="24"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B100" s="28"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="28"/>
+      <c r="E100" s="28"/>
+      <c r="F100" s="28"/>
+      <c r="G100" s="28"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>334</v>
       </c>
@@ -7176,17 +7180,20 @@
       <c r="D101" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E101" s="29" t="s">
+      <c r="E101" s="23" t="s">
         <v>365</v>
       </c>
-      <c r="F101" s="29" t="s">
+      <c r="F101" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="G101" s="29" t="s">
+      <c r="G101" s="23" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H101" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>335</v>
       </c>
@@ -7197,30 +7204,30 @@
       <c r="D102" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E102" s="29" t="s">
+      <c r="E102" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="F102" s="29" t="s">
+      <c r="F102" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G102" s="29" t="s">
+      <c r="G102" s="23" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="22" t="s">
+    <row r="103" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="30" t="s">
         <v>342</v>
       </c>
-      <c r="B103" s="22"/>
-      <c r="C103" s="22"/>
-      <c r="D103" s="22"/>
+      <c r="B103" s="30"/>
+      <c r="C103" s="30"/>
+      <c r="D103" s="30"/>
       <c r="E103" s="43" t="s">
         <v>342</v>
       </c>
       <c r="F103" s="43"/>
       <c r="G103" s="43"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>322</v>
       </c>
@@ -7231,17 +7238,17 @@
       <c r="D104" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E104" s="29" t="s">
+      <c r="E104" s="23" t="s">
         <v>403</v>
       </c>
-      <c r="F104" s="29" t="s">
+      <c r="F104" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="G104" s="29" t="s">
+      <c r="G104" s="23" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>325</v>
       </c>
@@ -7252,41 +7259,41 @@
       <c r="D105" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E105" s="29" t="s">
+      <c r="E105" s="23" t="s">
         <v>360</v>
       </c>
-      <c r="F105" s="29" t="s">
+      <c r="F105" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="G105" s="29" t="s">
+      <c r="G105" s="23" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="24" t="s">
+    <row r="106" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="28" t="s">
         <v>402</v>
       </c>
-      <c r="B106" s="24"/>
-      <c r="C106" s="24"/>
-      <c r="D106" s="24"/>
-      <c r="E106" s="24"/>
-      <c r="F106" s="24"/>
-      <c r="G106" s="24"/>
-    </row>
-    <row r="107" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="22" t="s">
+      <c r="B106" s="28"/>
+      <c r="C106" s="28"/>
+      <c r="D106" s="28"/>
+      <c r="E106" s="28"/>
+      <c r="F106" s="28"/>
+      <c r="G106" s="28"/>
+    </row>
+    <row r="107" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="30" t="s">
         <v>406</v>
       </c>
-      <c r="B107" s="22"/>
-      <c r="C107" s="22"/>
-      <c r="D107" s="22"/>
-      <c r="E107" s="23" t="s">
+      <c r="B107" s="30"/>
+      <c r="C107" s="30"/>
+      <c r="D107" s="30"/>
+      <c r="E107" s="31" t="s">
         <v>405</v>
       </c>
-      <c r="F107" s="23"/>
-      <c r="G107" s="23"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F107" s="31"/>
+      <c r="G107" s="31"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>400</v>
       </c>
@@ -7297,17 +7304,17 @@
       <c r="D108" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E108" s="29" t="s">
+      <c r="E108" s="23" t="s">
         <v>365</v>
       </c>
-      <c r="F108" s="29" t="s">
+      <c r="F108" s="23" t="s">
         <v>365</v>
       </c>
-      <c r="G108" s="29" t="s">
+      <c r="G108" s="23" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>401</v>
       </c>
@@ -7318,30 +7325,30 @@
       <c r="D109" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E109" s="29" t="s">
+      <c r="E109" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="F109" s="29" t="s">
+      <c r="F109" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G109" s="29" t="s">
+      <c r="G109" s="23" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="22" t="s">
+    <row r="110" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="30" t="s">
         <v>408</v>
       </c>
-      <c r="B110" s="22"/>
-      <c r="C110" s="22"/>
-      <c r="D110" s="22"/>
-      <c r="E110" s="23" t="s">
+      <c r="B110" s="30"/>
+      <c r="C110" s="30"/>
+      <c r="D110" s="30"/>
+      <c r="E110" s="31" t="s">
         <v>407</v>
       </c>
-      <c r="F110" s="23"/>
-      <c r="G110" s="23"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F110" s="31"/>
+      <c r="G110" s="31"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>400</v>
       </c>
@@ -7352,17 +7359,17 @@
       <c r="D111" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E111" s="29" t="s">
+      <c r="E111" s="23" t="s">
         <v>364</v>
       </c>
-      <c r="F111" s="29" t="s">
+      <c r="F111" s="23" t="s">
         <v>364</v>
       </c>
-      <c r="G111" s="29" t="s">
+      <c r="G111" s="23" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>401</v>
       </c>
@@ -7373,28 +7380,28 @@
       <c r="D112" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E112" s="29" t="s">
+      <c r="E112" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="F112" s="29" t="s">
+      <c r="F112" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G112" s="29" t="s">
+      <c r="G112" s="23" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="22" t="s">
+      <c r="A113" s="30" t="s">
         <v>412</v>
       </c>
-      <c r="B113" s="22"/>
-      <c r="C113" s="22"/>
-      <c r="D113" s="22"/>
-      <c r="E113" s="23" t="s">
+      <c r="B113" s="30"/>
+      <c r="C113" s="30"/>
+      <c r="D113" s="30"/>
+      <c r="E113" s="31" t="s">
         <v>411</v>
       </c>
-      <c r="F113" s="23"/>
-      <c r="G113" s="23"/>
+      <c r="F113" s="31"/>
+      <c r="G113" s="31"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
@@ -7407,13 +7414,13 @@
       <c r="D114" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E114" s="29" t="s">
+      <c r="E114" s="23" t="s">
         <v>365</v>
       </c>
-      <c r="F114" s="29" t="s">
+      <c r="F114" s="23" t="s">
         <v>365</v>
       </c>
-      <c r="G114" s="29" t="s">
+      <c r="G114" s="23" t="s">
         <v>385</v>
       </c>
     </row>
@@ -7428,80 +7435,79 @@
       <c r="D115" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E115" s="29" t="s">
+      <c r="E115" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="F115" s="29" t="s">
+      <c r="F115" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G115" s="29" t="s">
+      <c r="G115" s="23" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A116" s="24" t="s">
+      <c r="A116" s="28" t="s">
         <v>348</v>
       </c>
-      <c r="B116" s="24"/>
-      <c r="C116" s="24"/>
-      <c r="D116" s="24"/>
-      <c r="E116" s="24"/>
-      <c r="F116" s="24"/>
-      <c r="G116" s="24"/>
+      <c r="B116" s="28"/>
+      <c r="C116" s="28"/>
+      <c r="D116" s="28"/>
+      <c r="E116" s="28"/>
+      <c r="F116" s="28"/>
+      <c r="G116" s="28"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A117" s="24" t="s">
+      <c r="A117" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="B117" s="24"/>
-      <c r="C117" s="24"/>
-      <c r="D117" s="24"/>
-      <c r="E117" s="24"/>
-      <c r="F117" s="24"/>
-      <c r="G117" s="24"/>
+      <c r="B117" s="28"/>
+      <c r="C117" s="28"/>
+      <c r="D117" s="28"/>
+      <c r="E117" s="28"/>
+      <c r="F117" s="28"/>
+      <c r="G117" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="A106:G106"/>
-    <mergeCell ref="A84:G84"/>
-    <mergeCell ref="A88:G88"/>
-    <mergeCell ref="A92:G92"/>
-    <mergeCell ref="A96:G96"/>
-    <mergeCell ref="A100:G100"/>
-    <mergeCell ref="F91:G91"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="E107:G107"/>
-    <mergeCell ref="A110:D110"/>
-    <mergeCell ref="E110:G110"/>
-    <mergeCell ref="A113:D113"/>
-    <mergeCell ref="E113:G113"/>
-    <mergeCell ref="A99:D99"/>
-    <mergeCell ref="A103:D103"/>
-    <mergeCell ref="E103:G103"/>
-    <mergeCell ref="E83:G83"/>
-    <mergeCell ref="A87:D87"/>
-    <mergeCell ref="E87:G87"/>
-    <mergeCell ref="A91:D91"/>
-    <mergeCell ref="A95:D95"/>
-    <mergeCell ref="E95:G95"/>
-    <mergeCell ref="A117:G117"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A116:G116"/>
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="E46:G46"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A74:D74"/>
     <mergeCell ref="E74:G74"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="A77:G77"/>
     <mergeCell ref="A68:D68"/>
     <mergeCell ref="E68:G68"/>
     <mergeCell ref="A71:D71"/>
@@ -7512,43 +7518,44 @@
     <mergeCell ref="E62:G62"/>
     <mergeCell ref="A65:D65"/>
     <mergeCell ref="E65:G65"/>
+    <mergeCell ref="A117:G117"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A116:G116"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="A77:G77"/>
     <mergeCell ref="A50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="E53:G53"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E83:G83"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A95:D95"/>
+    <mergeCell ref="E95:G95"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="E107:G107"/>
+    <mergeCell ref="A110:D110"/>
+    <mergeCell ref="E110:G110"/>
+    <mergeCell ref="A113:D113"/>
+    <mergeCell ref="E113:G113"/>
+    <mergeCell ref="A106:G106"/>
+    <mergeCell ref="A84:G84"/>
+    <mergeCell ref="A88:G88"/>
+    <mergeCell ref="A92:G92"/>
+    <mergeCell ref="A96:G96"/>
+    <mergeCell ref="A100:G100"/>
+    <mergeCell ref="F91:G91"/>
+    <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="E103:G103"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>